<commit_message>
Add block parameter in print_doc_block.
</commit_message>
<xml_diff>
--- a/abc.xlsx
+++ b/abc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ZhangZhihua\git\RegisterPrinter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Data\git\RegisterPrinter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF0D61E-BFB0-4EE3-B3A5-DD2A1C329C75}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F0EAFB3-668F-4396-AC8E-1A56B8B1AE62}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="1050" windowWidth="16965" windowHeight="11850" xr2:uid="{5A6D0F3A-115B-4AFB-A61C-6C0A1FFDE0E4}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14595" xr2:uid="{5A6D0F3A-115B-4AFB-A61C-6C0A1FFDE0E4}"/>
   </bookViews>
   <sheets>
     <sheet name="Top" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Top</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -86,6 +86,22 @@
   </si>
   <si>
     <t>Top_Module</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Instance3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Type1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x20000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x10000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -450,19 +466,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5B7D94AB-E61B-4C28-B4D2-B77B67645C4F}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.9" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -470,7 +486,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -478,7 +494,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -486,7 +502,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -494,7 +510,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -502,7 +518,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -516,7 +532,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -534,11 +550,25 @@
       </c>
       <c r="F9">
         <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>